<commit_message>
Completanto a informação do Excel
</commit_message>
<xml_diff>
--- a/Relatorio do Grupo.xlsx
+++ b/Relatorio do Grupo.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artur\Desktop\cTESP\Web\Cliente\Projeto_WEB_Last_FM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zé\Documents\Git\Projeto_WEB_Last_FM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B479E3-5588-4D7C-B6A4-240321130691}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFBFD94C-6884-4BC9-91E1-78E0F94C0C91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="60ON3kjtWffjZ7cCgAEBaxJHbrdNpkgzoot33jfiAkSmy4unfK1v6COADyhJeQq4ugrQvfaR8vJsny8BjjaGgw==" workbookSaltValue="oz6aXzV2VpdpS44VFlxigg==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Relatório Projeto - PWebCliente" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>Elementos do Grupo:</t>
   </si>
@@ -345,12 +345,6 @@
     <t>Não completo porque ao selecionar uma musica, não redericiona para os detalhes.</t>
   </si>
   <si>
-    <t xml:space="preserve">pagina index </t>
-  </si>
-  <si>
-    <t>menu está no header</t>
-  </si>
-  <si>
     <t>Não completo porque ao selecionar uma musica, não redericiona para os detalhes. Barra de pesquisa esta no header, e quando se submete pra pesquisar algo e esse query de pesquisa não é encotrado a pagina não avanca</t>
   </si>
   <si>
@@ -360,19 +354,28 @@
     <t>tem a imagem do album, nome artista, faixa e nome do album, e ainda uma seccao se houver de wiki.</t>
   </si>
   <si>
-    <t>Foi utilizado corretamente</t>
-  </si>
-  <si>
-    <t>É guardada dados, detalhes, favoritos</t>
-  </si>
-  <si>
     <t>Tem distinção, mas tem codigo que está repetido em funções. Podia estar melhor</t>
   </si>
   <si>
     <t>Sim foi corretamente utilizado o Git.</t>
   </si>
   <si>
-    <t>A pagina está completamente responsiva, menos as secoes de slideshow</t>
+    <t>O header esta disponivel em todas as páginas e ainda é chamado atravez de javascript</t>
+  </si>
+  <si>
+    <t>a homepage apresenta as 10 músicas mas não são chamadas, do top 10 portugal, nem dos favoritos</t>
+  </si>
+  <si>
+    <t>Utilizamos a API LastFM de acordo com a documentação disponiblizada</t>
+  </si>
+  <si>
+    <t>É armazenada toada a informação dos detalhes, favoritos e outros dados em uma LocalStorage</t>
+  </si>
+  <si>
+    <t>A pagina está completamente responsiva, menos as secoes de slideshow e o footer</t>
+  </si>
+  <si>
+    <t>Foi feita de forma clara e estruturada a informação, tanto como o design do site, simples assim dando um aspeto agradavel ao utilizador</t>
   </si>
 </sst>
 </file>
@@ -796,73 +799,76 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -890,11 +896,8 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2055,8 +2058,8 @@
   <dimension ref="B2:I69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21:I21"/>
+      <pane ySplit="12" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F63" sqref="F63:I63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2114,28 +2117,28 @@
       <c r="I6" s="9"/>
     </row>
     <row r="7" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
     </row>
     <row r="8" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
     </row>
     <row r="9" spans="2:9" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9"/>
@@ -2152,12 +2155,12 @@
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="47">
+      <c r="C11" s="48">
         <v>203</v>
       </c>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="50"/>
       <c r="I11" s="2" t="s">
         <v>30</v>
       </c>
@@ -2168,16 +2171,16 @@
       </c>
     </row>
     <row r="13" spans="2:9" ht="25.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="2:9" ht="10.050000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="11"/>
@@ -2199,12 +2202,12 @@
       <c r="E15" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="50" t="s">
+      <c r="F15" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="53"/>
     </row>
     <row r="16" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
@@ -2216,12 +2219,12 @@
       <c r="E16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="50" t="s">
+      <c r="F16" s="51" t="s">
         <v>60</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="53"/>
     </row>
     <row r="17" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
@@ -2233,80 +2236,80 @@
       <c r="E17" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="50" t="s">
+      <c r="F17" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="51"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="53"/>
     </row>
     <row r="18" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
     </row>
     <row r="19" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
     </row>
     <row r="20" spans="2:9" s="12" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
     </row>
     <row r="21" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
     </row>
     <row r="22" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
+      <c r="B22" s="44"/>
+      <c r="C22" s="44"/>
+      <c r="D22" s="44"/>
+      <c r="E22" s="44"/>
+      <c r="F22" s="44"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="44"/>
+      <c r="I22" s="44"/>
     </row>
     <row r="23" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
     </row>
     <row r="24" spans="2:9" s="12" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="13" t="s">
@@ -2317,64 +2320,64 @@
       <c r="E24" s="20"/>
     </row>
     <row r="25" spans="2:9" ht="58.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="27"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
     </row>
     <row r="27" spans="2:9" ht="19.95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
     </row>
     <row r="28" spans="2:9" s="12" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="41"/>
-      <c r="I28" s="41"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
     </row>
     <row r="29" spans="2:9" ht="58.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
+      <c r="B29" s="46"/>
+      <c r="C29" s="46"/>
+      <c r="D29" s="46"/>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
     </row>
     <row r="30" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
     </row>
     <row r="31" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="40" t="s">
+      <c r="B31" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
     </row>
     <row r="32" spans="2:9" s="12" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="13" t="s">
@@ -2385,14 +2388,14 @@
       <c r="E32" s="20"/>
     </row>
     <row r="33" spans="2:9" ht="58.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="27"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
-      <c r="G33" s="27"/>
-      <c r="H33" s="27"/>
-      <c r="I33" s="27"/>
+      <c r="B33" s="46"/>
+      <c r="C33" s="46"/>
+      <c r="D33" s="46"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
     </row>
     <row r="34" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="23"/>
@@ -2405,218 +2408,218 @@
       <c r="I34" s="23"/>
     </row>
     <row r="36" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="26" t="s">
+      <c r="B36" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="26"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="26"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="26"/>
-      <c r="I36" s="26"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="42"/>
+      <c r="G36" s="42"/>
+      <c r="H36" s="42"/>
+      <c r="I36" s="42"/>
     </row>
     <row r="37" spans="2:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="37"/>
-      <c r="D37" s="37"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="37"/>
-      <c r="G37" s="37"/>
-      <c r="H37" s="37"/>
-      <c r="I37" s="37"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
     </row>
     <row r="38" spans="2:9" ht="13.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="37"/>
-      <c r="C38" s="37"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="37"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="37"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="37"/>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
     </row>
     <row r="39" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="30" t="s">
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="31"/>
+      <c r="G39" s="32"/>
+      <c r="H39" s="32"/>
+      <c r="I39" s="33"/>
     </row>
     <row r="40" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="39"/>
-      <c r="C40" s="32" t="s">
+      <c r="B40" s="29"/>
+      <c r="C40" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D40" s="33"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="35" t="s">
+      <c r="D40" s="35"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G40" s="37"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="38"/>
+    </row>
+    <row r="41" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="33"/>
+    </row>
+    <row r="42" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="29"/>
+      <c r="C42" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" s="35"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="37"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="38"/>
+    </row>
+    <row r="43" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="33"/>
+    </row>
+    <row r="44" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B44" s="29"/>
+      <c r="C44" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="35"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="G44" s="37"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="38"/>
+    </row>
+    <row r="45" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B45" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C45" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="33"/>
+    </row>
+    <row r="46" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="29"/>
+      <c r="C46" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D46" s="35"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G40" s="35"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-    </row>
-    <row r="41" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="29"/>
-      <c r="E41" s="29"/>
-      <c r="F41" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="31"/>
-    </row>
-    <row r="42" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="39"/>
-      <c r="C42" s="32" t="s">
+      <c r="G46" s="37"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="38"/>
+    </row>
+    <row r="47" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
+      <c r="I47" s="33"/>
+    </row>
+    <row r="48" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="29"/>
+      <c r="C48" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="35"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="G48" s="37"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="38"/>
+    </row>
+    <row r="49" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="G49" s="32"/>
+      <c r="H49" s="32"/>
+      <c r="I49" s="33"/>
+    </row>
+    <row r="50" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="29"/>
+      <c r="C50" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D42" s="33"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="G42" s="35"/>
-      <c r="H42" s="35"/>
-      <c r="I42" s="36"/>
-    </row>
-    <row r="43" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="D43" s="29"/>
-      <c r="E43" s="29"/>
-      <c r="F43" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="31"/>
-    </row>
-    <row r="44" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B44" s="39"/>
-      <c r="C44" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D44" s="33"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="35" t="s">
+      <c r="D50" s="35"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="36"/>
-    </row>
-    <row r="45" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="38" t="s">
-        <v>24</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-      <c r="F45" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="G45" s="30"/>
-      <c r="H45" s="30"/>
-      <c r="I45" s="31"/>
-    </row>
-    <row r="46" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="39"/>
-      <c r="C46" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D46" s="33"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="G46" s="35"/>
-      <c r="H46" s="35"/>
-      <c r="I46" s="36"/>
-    </row>
-    <row r="47" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="D47" s="29"/>
-      <c r="E47" s="29"/>
-      <c r="F47" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="31"/>
-    </row>
-    <row r="48" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B48" s="39"/>
-      <c r="C48" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="33"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="G48" s="35"/>
-      <c r="H48" s="35"/>
-      <c r="I48" s="36"/>
-    </row>
-    <row r="49" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B49" s="38" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-      <c r="F49" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="G49" s="30"/>
-      <c r="H49" s="30"/>
-      <c r="I49" s="31"/>
-    </row>
-    <row r="50" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="39"/>
-      <c r="C50" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D50" s="33"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="G50" s="35"/>
-      <c r="H50" s="35"/>
-      <c r="I50" s="36"/>
+      <c r="G50" s="37"/>
+      <c r="H50" s="37"/>
+      <c r="I50" s="38"/>
     </row>
     <row r="51" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="5"/>
@@ -2629,216 +2632,218 @@
       <c r="I51" s="25"/>
     </row>
     <row r="53" spans="2:9" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C53" s="53"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="53"/>
-      <c r="F53" s="53"/>
-      <c r="G53" s="53"/>
-      <c r="H53" s="53"/>
-      <c r="I53" s="53"/>
+      <c r="C53" s="39"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="39"/>
+      <c r="H53" s="39"/>
+      <c r="I53" s="39"/>
     </row>
     <row r="54" spans="2:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B54" s="37" t="s">
+      <c r="B54" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="37"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="G54" s="27"/>
+      <c r="H54" s="27"/>
+      <c r="I54" s="27"/>
     </row>
     <row r="55" spans="2:9" ht="13.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="37"/>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="27"/>
+      <c r="E55" s="27"/>
+      <c r="F55" s="27"/>
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="I55" s="27"/>
     </row>
     <row r="56" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B56" s="38" t="s">
+      <c r="B56" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C56" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="D56" s="29"/>
-      <c r="E56" s="29"/>
-      <c r="F56" s="30" t="s">
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
-      <c r="I56" s="31"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
+      <c r="I56" s="33"/>
     </row>
     <row r="57" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="39"/>
-      <c r="C57" s="32" t="s">
+      <c r="B57" s="29"/>
+      <c r="C57" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D57" s="33"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="G57" s="35"/>
-      <c r="H57" s="35"/>
-      <c r="I57" s="36"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="G57" s="37"/>
+      <c r="H57" s="37"/>
+      <c r="I57" s="38"/>
     </row>
     <row r="58" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B58" s="38" t="s">
+      <c r="B58" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C58" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D58" s="29"/>
-      <c r="E58" s="29"/>
-      <c r="F58" s="30" t="s">
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="31"/>
+      <c r="G58" s="32"/>
+      <c r="H58" s="32"/>
+      <c r="I58" s="33"/>
     </row>
     <row r="59" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B59" s="39"/>
-      <c r="C59" s="32" t="s">
+      <c r="B59" s="29"/>
+      <c r="C59" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D59" s="33"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="G59" s="35"/>
-      <c r="H59" s="35"/>
-      <c r="I59" s="36"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="36"/>
+      <c r="F59" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
+      <c r="I59" s="38"/>
     </row>
     <row r="60" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="38" t="s">
+      <c r="B60" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="D60" s="29"/>
-      <c r="E60" s="29"/>
-      <c r="F60" s="30" t="s">
+      <c r="D60" s="31"/>
+      <c r="E60" s="31"/>
+      <c r="F60" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="31"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="33"/>
     </row>
     <row r="61" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B61" s="39"/>
-      <c r="C61" s="32" t="s">
+      <c r="B61" s="29"/>
+      <c r="C61" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D61" s="33"/>
-      <c r="E61" s="34"/>
-      <c r="F61" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="G61" s="35"/>
-      <c r="H61" s="35"/>
-      <c r="I61" s="36"/>
+      <c r="D61" s="35"/>
+      <c r="E61" s="36"/>
+      <c r="F61" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
+      <c r="I61" s="38"/>
     </row>
     <row r="62" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="38" t="s">
+      <c r="B62" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C62" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D62" s="29"/>
-      <c r="E62" s="29"/>
-      <c r="F62" s="30" t="s">
+      <c r="D62" s="31"/>
+      <c r="E62" s="31"/>
+      <c r="F62" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="31"/>
+      <c r="G62" s="32"/>
+      <c r="H62" s="32"/>
+      <c r="I62" s="33"/>
     </row>
     <row r="63" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B63" s="39"/>
-      <c r="C63" s="32" t="s">
+      <c r="B63" s="29"/>
+      <c r="C63" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="35"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="38"/>
+    </row>
+    <row r="64" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C64" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D64" s="31"/>
+      <c r="E64" s="31"/>
+      <c r="F64" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="33"/>
+    </row>
+    <row r="65" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="29"/>
+      <c r="C65" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="D63" s="33"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="35"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="36"/>
-    </row>
-    <row r="64" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="38" t="s">
-        <v>46</v>
-      </c>
-      <c r="C64" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D64" s="29"/>
-      <c r="E64" s="29"/>
-      <c r="F64" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="31"/>
-    </row>
-    <row r="65" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="39"/>
-      <c r="C65" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="D65" s="33"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="35" t="s">
+      <c r="D65" s="35"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="G65" s="35"/>
-      <c r="H65" s="35"/>
-      <c r="I65" s="36"/>
+      <c r="G65" s="37"/>
+      <c r="H65" s="37"/>
+      <c r="I65" s="38"/>
     </row>
     <row r="66" spans="2:9" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="38" t="s">
+      <c r="B66" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="C66" s="28" t="s">
+      <c r="C66" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="D66" s="29"/>
-      <c r="E66" s="29"/>
-      <c r="F66" s="30" t="s">
+      <c r="D66" s="31"/>
+      <c r="E66" s="31"/>
+      <c r="F66" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="G66" s="30"/>
-      <c r="H66" s="30"/>
-      <c r="I66" s="31"/>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
+      <c r="I66" s="33"/>
     </row>
     <row r="67" spans="2:9" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B67" s="39"/>
-      <c r="C67" s="32" t="s">
+      <c r="B67" s="29"/>
+      <c r="C67" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="D67" s="33"/>
-      <c r="E67" s="34"/>
-      <c r="F67" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="G67" s="35"/>
-      <c r="H67" s="35"/>
-      <c r="I67" s="36"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G67" s="37"/>
+      <c r="H67" s="37"/>
+      <c r="I67" s="38"/>
     </row>
     <row r="68" spans="2:9" s="4" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C68" s="21"/>
@@ -2846,20 +2851,90 @@
       <c r="E68" s="21"/>
     </row>
     <row r="69" spans="2:9" s="14" customFormat="1" ht="43.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C69" s="54"/>
-      <c r="D69" s="54"/>
-      <c r="E69" s="54"/>
-      <c r="F69" s="54"/>
-      <c r="G69" s="54"/>
-      <c r="H69" s="54"/>
-      <c r="I69" s="54"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="26"/>
+      <c r="I69" s="26"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="UXNnFf7ebbUNogGNRojvI7glYLJEGRyjKKG/sHLA135X6CzInlVlMlKuhI7d4CQFWx6dgEa6QZh9okcL11ex2w==" saltValue="49Vxi4VJp1JBxZNWkxPUow==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertHyperlinks="0" selectLockedCells="1"/>
   <mergeCells count="86">
+    <mergeCell ref="B36:I36"/>
+    <mergeCell ref="B33:I33"/>
+    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="C43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="B38:I38"/>
+    <mergeCell ref="B37:I37"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="C42:E42"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="F17:I17"/>
+    <mergeCell ref="C67:E67"/>
+    <mergeCell ref="F67:I67"/>
+    <mergeCell ref="C66:E66"/>
+    <mergeCell ref="F66:I66"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="F60:I60"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="F61:I61"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="B53:I53"/>
     <mergeCell ref="B69:I69"/>
     <mergeCell ref="B54:I54"/>
     <mergeCell ref="B55:I55"/>
@@ -2876,76 +2951,6 @@
     <mergeCell ref="F63:I63"/>
     <mergeCell ref="B60:B61"/>
     <mergeCell ref="C60:E60"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="B53:I53"/>
-    <mergeCell ref="C67:E67"/>
-    <mergeCell ref="F67:I67"/>
-    <mergeCell ref="C66:E66"/>
-    <mergeCell ref="F66:I66"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="F60:I60"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="F61:I61"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="B18:I18"/>
-    <mergeCell ref="B19:I19"/>
-    <mergeCell ref="B21:I21"/>
-    <mergeCell ref="B20:I20"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F17:I17"/>
-    <mergeCell ref="B27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="B25:I25"/>
-    <mergeCell ref="B29:I29"/>
-    <mergeCell ref="B31:I31"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="B36:I36"/>
-    <mergeCell ref="B33:I33"/>
-    <mergeCell ref="C49:E49"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="C43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="B38:I38"/>
-    <mergeCell ref="B37:I37"/>
-    <mergeCell ref="B56:B57"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="C39:E40">

</xml_diff>